<commit_message>
observacao e fonte adicionado no arquivo de upload
</commit_message>
<xml_diff>
--- a/t/user/teste-upload.xlsx
+++ b/t/user/teste-upload.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>variavel id</t>
   </si>
@@ -38,12 +38,21 @@
     <t>ignoradas</t>
   </si>
   <si>
+    <t>fonte</t>
+  </si>
+  <si>
+    <t>observacao</t>
+  </si>
+  <si>
     <t>popoulacao</t>
   </si>
   <si>
     <t>asdasd</t>
   </si>
   <si>
+    <t>isso eh uma fonte</t>
+  </si>
+  <si>
     <t>xxx</t>
   </si>
   <si>
@@ -51,6 +60,12 @@
   </si>
   <si>
     <t>aaa</t>
+  </si>
+  <si>
+    <t>segunda fonte</t>
+  </si>
+  <si>
+    <t>alguma obs</t>
   </si>
 </sst>
 </file>
@@ -126,8 +141,9 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -146,14 +162,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
+      <selection activeCell="H1" activeCellId="0" pane="topLeft" sqref="H1:I4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -178,30 +194,40 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>40940</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2013</v>
@@ -210,27 +236,35 @@
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>3333333333</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>42006</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>655</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tratar encoding do XLS e XLSx
</commit_message>
<xml_diff>
--- a/t/user/teste-upload.xlsx
+++ b/t/user/teste-upload.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>variavel id</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>xxx</t>
+  </si>
+  <si>
+    <t>puntuação</t>
   </si>
   <si>
     <t>xx</t>
@@ -165,11 +168,11 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H1" activeCellId="0" pane="topLeft" sqref="H1:I4"/>
+      <selection activeCell="H3" activeCellId="0" pane="topLeft" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -241,7 +244,9 @@
       <c r="F3" s="0" t="n">
         <v>3333333333</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I3" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
@@ -249,7 +254,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>42006</v>
@@ -258,13 +263,13 @@
         <v>655</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>